<commit_message>
Add Process Flow View with error handling and loading functionality
- Introduced a new 'Process Flow' view in the application, allowing users to visualize horizontal dependencies between L3 processes.
- Added buttons for loading files, zooming in/out, fitting to screen, and resetting zoom.
- Implemented error handling for loading process flow data, providing user guidance in case of issues.
- Removed the outdated Hierarchy.xlsx file to streamline data management.
</commit_message>
<xml_diff>
--- a/SCE AMI - Process Hierarchy.xlsx
+++ b/SCE AMI - Process Hierarchy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus.sharepoint.com/sites/SCEPursuitTeam/Shared Documents/AMI 2.0 OCM PMO RFP/7 - Oral Presentation Rd 2/BRD Artifacts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/tony_calabro_ey_com/Documents/Desktop/Cursor/Hierarchy 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="776" documentId="8_{D0A48B66-DD14-4E33-BEEA-FA64DE0E4EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AAF7B64-D9F9-46E6-9284-DC50927ADA1D}"/>
+  <xr:revisionPtr revIDLastSave="777" documentId="8_{D0A48B66-DD14-4E33-BEEA-FA64DE0E4EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C13B03FF-F6C1-4D4B-99FF-566F4D3F79A7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5CF7D8D-18C1-4DA6-BBC5-CBC3C1BDFBAD}"/>
   </bookViews>
@@ -2529,7 +2529,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2588,13 +2588,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="EYInterstate Light"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2701,7 +2694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2755,12 +2748,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4315,8 +4302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8892926-E8FC-4E51-8265-E6D97D7EE353}">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4494,7 +4481,7 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -4757,7 +4744,7 @@
       <c r="C17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="18" t="s">
         <v>664</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -4835,7 +4822,7 @@
       <c r="C20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="18" t="s">
         <v>665</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -4861,7 +4848,7 @@
       <c r="C21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="18" t="s">
         <v>666</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -4887,7 +4874,7 @@
       <c r="C22" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>667</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -4903,7 +4890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>62</v>
       </c>
@@ -4913,7 +4900,7 @@
       <c r="C23" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="18" t="s">
         <v>668</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -5017,7 +5004,7 @@
       <c r="C27" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>669</v>
       </c>
       <c r="E27" s="11" t="s">
@@ -5043,7 +5030,7 @@
       <c r="C28" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>670</v>
       </c>
       <c r="E28" s="11" t="s">
@@ -5069,7 +5056,7 @@
       <c r="C29" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="18" t="s">
         <v>671</v>
       </c>
       <c r="E29" s="11" t="s">
@@ -5095,7 +5082,7 @@
       <c r="C30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="18" t="s">
         <v>672</v>
       </c>
       <c r="E30" s="11" t="s">
@@ -5121,7 +5108,7 @@
       <c r="C31" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="18" t="s">
         <v>673</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -5147,7 +5134,7 @@
       <c r="C32" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="18" t="s">
         <v>674</v>
       </c>
       <c r="E32" s="11" t="s">
@@ -5173,7 +5160,7 @@
       <c r="C33" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="18" t="s">
         <v>675</v>
       </c>
       <c r="E33" s="11" t="s">
@@ -5303,7 +5290,7 @@
       <c r="C38" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="18" t="s">
         <v>676</v>
       </c>
       <c r="E38" s="11" t="s">
@@ -5433,7 +5420,7 @@
       <c r="C43" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="18" t="s">
         <v>677</v>
       </c>
       <c r="E43" s="11" t="s">
@@ -5459,7 +5446,7 @@
       <c r="C44" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="18" t="s">
         <v>678</v>
       </c>
       <c r="E44" s="11" t="s">
@@ -5563,7 +5550,7 @@
       <c r="C48" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="18" t="s">
         <v>679</v>
       </c>
       <c r="E48" s="11" t="s">
@@ -5719,7 +5706,7 @@
       <c r="C54" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="20" t="s">
+      <c r="D54" s="18" t="s">
         <v>680</v>
       </c>
       <c r="E54" s="11" t="s">
@@ -5745,7 +5732,7 @@
       <c r="C55" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="18" t="s">
         <v>681</v>
       </c>
       <c r="E55" s="11" t="s">
@@ -5771,7 +5758,7 @@
       <c r="C56" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="D56" s="11" t="s">
         <v>682</v>
       </c>
       <c r="E56" s="11" t="s">
@@ -5797,7 +5784,7 @@
       <c r="C57" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="11" t="s">
         <v>683</v>
       </c>
       <c r="E57" s="11" t="s">
@@ -5875,7 +5862,7 @@
       <c r="C60" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D60" s="11" t="s">
         <v>684</v>
       </c>
       <c r="E60" s="11" t="s">
@@ -5953,7 +5940,7 @@
       <c r="C63" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D63" s="21" t="s">
+      <c r="D63" s="11" t="s">
         <v>685</v>
       </c>
       <c r="E63" s="11" t="s">
@@ -5979,7 +5966,7 @@
       <c r="C64" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D64" s="21" t="s">
+      <c r="D64" s="11" t="s">
         <v>686</v>
       </c>
       <c r="E64" s="11" t="s">
@@ -6057,7 +6044,7 @@
       <c r="C67" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D67" s="21" t="s">
+      <c r="D67" s="11" t="s">
         <v>705</v>
       </c>
       <c r="E67" s="11" t="s">
@@ -6083,7 +6070,7 @@
       <c r="C68" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="D68" s="21" t="s">
+      <c r="D68" s="11" t="s">
         <v>704</v>
       </c>
       <c r="E68" s="11" t="s">
@@ -6109,7 +6096,7 @@
       <c r="C69" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="D69" s="21" t="s">
+      <c r="D69" s="11" t="s">
         <v>703</v>
       </c>
       <c r="E69" s="11" t="s">
@@ -6187,7 +6174,7 @@
       <c r="C72" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="D72" s="21" t="s">
+      <c r="D72" s="11" t="s">
         <v>702</v>
       </c>
       <c r="E72" s="11" t="s">
@@ -6213,7 +6200,7 @@
       <c r="C73" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D73" s="21" t="s">
+      <c r="D73" s="11" t="s">
         <v>701</v>
       </c>
       <c r="E73" s="11" t="s">
@@ -6239,7 +6226,7 @@
       <c r="C74" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="D74" s="21" t="s">
+      <c r="D74" s="11" t="s">
         <v>700</v>
       </c>
       <c r="E74" s="11" t="s">
@@ -6447,7 +6434,7 @@
       <c r="C82" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="D82" s="21" t="s">
+      <c r="D82" s="11" t="s">
         <v>699</v>
       </c>
       <c r="E82" s="11" t="s">
@@ -6473,7 +6460,7 @@
       <c r="C83" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="D83" s="21" t="s">
+      <c r="D83" s="11" t="s">
         <v>698</v>
       </c>
       <c r="E83" s="11" t="s">
@@ -6541,7 +6528,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>184</v>
       </c>
@@ -6551,7 +6538,7 @@
       <c r="C86" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="D86" s="21" t="s">
+      <c r="D86" s="11" t="s">
         <v>697</v>
       </c>
       <c r="E86" s="11" t="s">
@@ -6603,7 +6590,7 @@
       <c r="C88" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="D88" s="21" t="s">
+      <c r="D88" s="11" t="s">
         <v>696</v>
       </c>
       <c r="E88" s="11" t="s">
@@ -6629,7 +6616,7 @@
       <c r="C89" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="D89" s="21" t="s">
+      <c r="D89" s="11" t="s">
         <v>654</v>
       </c>
       <c r="E89" s="11" t="s">
@@ -6707,7 +6694,7 @@
       <c r="C92" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="D92" s="21" t="s">
+      <c r="D92" s="11" t="s">
         <v>695</v>
       </c>
       <c r="E92" s="11" t="s">
@@ -6781,7 +6768,7 @@
       <c r="C95" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="D95" s="21" t="s">
+      <c r="D95" s="11" t="s">
         <v>693</v>
       </c>
       <c r="E95" s="11" t="s">
@@ -6807,7 +6794,7 @@
       <c r="C96" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D96" s="21" t="s">
+      <c r="D96" s="11" t="s">
         <v>694</v>
       </c>
       <c r="E96" s="11" t="s">
@@ -6833,7 +6820,7 @@
       <c r="C97" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="D97" s="21" t="s">
+      <c r="D97" s="11" t="s">
         <v>692</v>
       </c>
       <c r="E97" s="11" t="s">
@@ -6859,7 +6846,7 @@
       <c r="C98" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="D98" s="21" t="s">
+      <c r="D98" s="11" t="s">
         <v>691</v>
       </c>
       <c r="E98" s="11" t="s">
@@ -6909,7 +6896,7 @@
       <c r="C100" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="D100" s="21" t="s">
+      <c r="D100" s="11" t="s">
         <v>690</v>
       </c>
       <c r="E100" s="11" t="s">
@@ -6935,7 +6922,7 @@
       <c r="C101" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="D101" s="21" t="s">
+      <c r="D101" s="11" t="s">
         <v>689</v>
       </c>
       <c r="E101" s="11" t="s">
@@ -7039,7 +7026,7 @@
       <c r="C105" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="D105" s="21" t="s">
+      <c r="D105" s="11" t="s">
         <v>688</v>
       </c>
       <c r="E105" s="11" t="s">
@@ -7065,7 +7052,7 @@
       <c r="C106" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="D106" s="21" t="s">
+      <c r="D106" s="11" t="s">
         <v>687</v>
       </c>
       <c r="E106" s="11" t="s">
@@ -11696,15 +11683,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFB9E5947890A84F90C1025035B3A9E9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0fe1b0914d5c8b09183d39f4cd0f7192">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="139fca70-673f-44e1-94c2-b523bb9c108c" xmlns:ns3="7eaf932d-7370-48c5-9459-ae540daf9d7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="356422204f896a562ca62bf92a067cf0" ns2:_="" ns3:_="">
     <xsd:import namespace="139fca70-673f-44e1-94c2-b523bb9c108c"/>
@@ -11911,6 +11889,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B57CF69-5D19-450C-935B-68EC43A8DA31}">
   <ds:schemaRefs>
@@ -11929,14 +11916,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB2BB8B-BA4E-4835-AC34-431A62162A7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42A97454-B7ED-4BA8-A1AC-B982151F7AF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11953,4 +11932,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB2BB8B-BA4E-4835-AC34-431A62162A7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>